<commit_message>
Add remaining features for Dietician creation
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dietician.xlsx
+++ b/src/test/resources/testdata/dietician.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>Firstname</t>
   </si>
@@ -43,50 +46,124 @@
     <t>HospitalCity</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>5234564890</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>trbda@gmail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>2013-05-22T18:14:08.570Z</t>
-  </si>
-  <si>
-    <t>Health and Science</t>
-  </si>
-  <si>
-    <t>Augustus</t>
-  </si>
-  <si>
-    <t>Parmer</t>
-  </si>
-  <si>
-    <t>787177</t>
-  </si>
-  <si>
-    <t>Kyle</t>
+    <t>JohnFull</t>
+  </si>
+  <si>
+    <t>DoeFull</t>
+  </si>
+  <si>
+    <t>1111111111</t>
+  </si>
+  <si>
+    <t>johndoefull@gmail.com</t>
+  </si>
+  <si>
+    <t>1901-01-01T01:01:01.111Z</t>
+  </si>
+  <si>
+    <t>Education 1</t>
+  </si>
+  <si>
+    <t>HospitalName 1</t>
+  </si>
+  <si>
+    <t>HospitalStreet 1</t>
+  </si>
+  <si>
+    <t>111111</t>
+  </si>
+  <si>
+    <t>HospitalCity 1</t>
+  </si>
+  <si>
+    <t>JohnMandatory</t>
+  </si>
+  <si>
+    <t>DoeMandatory</t>
+  </si>
+  <si>
+    <t>2222222222</t>
+  </si>
+  <si>
+    <t>johndoemandatory@gmail.com</t>
+  </si>
+  <si>
+    <t>1902-02-02T02:02:02.222Z</t>
+  </si>
+  <si>
+    <t>Education 2</t>
+  </si>
+  <si>
+    <t>HospitalName 2</t>
+  </si>
+  <si>
+    <t>HospitalStreet 2</t>
+  </si>
+  <si>
+    <t>222222</t>
+  </si>
+  <si>
+    <t>HospitalCity 2</t>
+  </si>
+  <si>
+    <t>3333333333</t>
+  </si>
+  <si>
+    <t>JohnAdditional</t>
+  </si>
+  <si>
+    <t>DoeAdditional</t>
+  </si>
+  <si>
+    <t>johndoeadditional@gmail.com</t>
+  </si>
+  <si>
+    <t>1903-03-03T03:03:03.333Z</t>
+  </si>
+  <si>
+    <t>Education 3</t>
+  </si>
+  <si>
+    <t>HospitalName 3</t>
+  </si>
+  <si>
+    <t>HospitalStreet 3</t>
+  </si>
+  <si>
+    <t>333333</t>
+  </si>
+  <si>
+    <t>HospitalCity 3</t>
+  </si>
+  <si>
+    <t>JohnInvalidPincode</t>
+  </si>
+  <si>
+    <t>DoeInvalidPincode</t>
+  </si>
+  <si>
+    <t>4444444444</t>
+  </si>
+  <si>
+    <t>johndoeinvalid@gmail.com</t>
+  </si>
+  <si>
+    <t>1904-04-04T04:04:04.444Z</t>
+  </si>
+  <si>
+    <t>Education 4</t>
+  </si>
+  <si>
+    <t>HospitalName 4</t>
+  </si>
+  <si>
+    <t>HospitalStreet 4</t>
+  </si>
+  <si>
+    <t>444444444444444444</t>
+  </si>
+  <si>
+    <t>HospitalCity 4</t>
   </si>
 </sst>
 </file>
@@ -96,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -114,12 +191,6 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -145,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -179,94 +250,37 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thin">
         <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -276,7 +290,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -289,32 +303,11 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -337,7 +330,6 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1372,23 +1364,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.1719" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.1719" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="2" width="12.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.3516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1719" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.1719" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1422,11 +1414,12 @@
       <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
+      <c r="K1" t="s" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>10</v>
-      </c>
+      <c r="A2" s="3"/>
       <c r="B2" t="s" s="3">
         <v>11</v>
       </c>
@@ -1454,107 +1447,112 @@
       <c r="J2" t="s" s="3">
         <v>19</v>
       </c>
+      <c r="K2" t="s" s="3">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" ht="14.7" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s" s="3">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" ht="14.7" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
+    <row r="4" ht="20.25" customHeight="1">
+      <c r="A4" t="s" s="4">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s" s="4">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s" s="4">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s" s="4">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s" s="4">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" ht="14.7" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
+    <row r="5" ht="20.25" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" t="s" s="5">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s" s="5">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s" s="5">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s" s="5">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s" s="5">
+        <v>48</v>
+      </c>
+      <c r="J5" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="K5" t="s" s="5">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display="trbda@gmail.com"/>
-  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>